<commit_message>
Se agrego autor del archivo
</commit_message>
<xml_diff>
--- a/EJERCICIOS.xlsx
+++ b/EJERCICIOS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875" tabRatio="818"/>
@@ -18,12 +18,15 @@
     <sheet name="ejercicio 8" sheetId="3" r:id="rId9"/>
     <sheet name="ejercicio 9" sheetId="1" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="161">
   <si>
     <t>Nombre</t>
   </si>
@@ -503,6 +506,9 @@
   </si>
   <si>
     <t>bound(A5,A9)</t>
+  </si>
+  <si>
+    <t>ALEJANDRO LOPEZ LUGO</t>
   </si>
 </sst>
 </file>
@@ -1748,21 +1754,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1784,12 +1775,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1799,7 +1833,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2085,17 +2119,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
         <v>128</v>
@@ -2282,14 +2321,14 @@
       <c r="E11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="104" t="s">
+      <c r="H11" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="125"/>
+      <c r="L11" s="125"/>
+      <c r="M11" s="125"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
@@ -2522,35 +2561,35 @@
       <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="104" t="s">
+      <c r="B26" s="125" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="125"/>
+      <c r="E26" s="125"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="125"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="125" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="104"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104"/>
+      <c r="C28" s="125"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="125"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2608,24 +2647,24 @@
       <selection activeCell="A34" sqref="A34:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="I2" s="107" t="s">
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="I2" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="106"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -2847,23 +2886,23 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="107"/>
-      <c r="H15" s="106" t="s">
+      <c r="C15" s="129"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="129"/>
+      <c r="H15" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="106"/>
-      <c r="O15" s="106"/>
-      <c r="P15" s="106"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="128"/>
+      <c r="M15" s="128"/>
+      <c r="N15" s="128"/>
+      <c r="O15" s="128"/>
+      <c r="P15" s="128"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -2882,11 +2921,11 @@
       <c r="F16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="108" t="s">
+      <c r="H16" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
       <c r="K16" s="30">
         <f>(C17*E17)+(C18*E18)+(C19*E19)+(C20*E20)+(C21*E21)</f>
         <v>28854</v>
@@ -2916,11 +2955,11 @@
       <c r="F17" s="23">
         <v>0</v>
       </c>
-      <c r="H17" s="108" t="s">
+      <c r="H17" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="108"/>
-      <c r="J17" s="108"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
       <c r="K17" s="30">
         <f>(F17*E17)+(F18*E18)+(F19*E19)+(F20*E20)+(F21*E21)</f>
         <v>27714</v>
@@ -2947,11 +2986,11 @@
       <c r="F18" s="24">
         <v>90</v>
       </c>
-      <c r="H18" s="108" t="s">
+      <c r="H18" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
       <c r="K18" s="30">
         <f>(C17*F17)+(C18*F18)+(C19*F19)+(C20*F20)+(C21*F21)</f>
         <v>27411</v>
@@ -2978,9 +3017,9 @@
       <c r="F19" s="23">
         <v>11</v>
       </c>
-      <c r="H19" s="104"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="104"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
       <c r="K19" s="6"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -3004,11 +3043,11 @@
       <c r="F20" s="24">
         <v>90</v>
       </c>
-      <c r="H20" s="104" t="s">
+      <c r="H20" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="104"/>
-      <c r="J20" s="104"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
       <c r="K20" s="32">
         <f>(2*K16)+(2*K17)-(2*K18)</f>
         <v>58314</v>
@@ -3035,24 +3074,24 @@
       <c r="F21" s="27">
         <v>101</v>
       </c>
-      <c r="H21" s="104" t="s">
+      <c r="H21" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
-      <c r="L21" s="104"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="104"/>
-      <c r="O21" s="104"/>
-      <c r="P21" s="104"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="125"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="104" t="s">
+      <c r="H22" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="104"/>
-      <c r="J22" s="104"/>
+      <c r="I22" s="125"/>
+      <c r="J22" s="125"/>
       <c r="K22" s="31">
         <f>(2*K16)+(2*K18)-(2*K17)</f>
         <v>57102</v>
@@ -3080,17 +3119,17 @@
       <c r="F23" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="104" t="s">
+      <c r="H23" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="104"/>
-      <c r="J23" s="104"/>
-      <c r="K23" s="104"/>
-      <c r="L23" s="104"/>
-      <c r="M23" s="104"/>
-      <c r="N23" s="104"/>
-      <c r="O23" s="104"/>
-      <c r="P23" s="104"/>
+      <c r="I23" s="125"/>
+      <c r="J23" s="125"/>
+      <c r="K23" s="125"/>
+      <c r="L23" s="125"/>
+      <c r="M23" s="125"/>
+      <c r="N23" s="125"/>
+      <c r="O23" s="125"/>
+      <c r="P23" s="125"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
@@ -3111,11 +3150,11 @@
       <c r="F24" s="3">
         <v>21</v>
       </c>
-      <c r="H24" s="104" t="s">
+      <c r="H24" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
+      <c r="I24" s="125"/>
+      <c r="J24" s="125"/>
       <c r="K24">
         <f>(2*K17)+(2*K16)-(2*K18)</f>
         <v>58314</v>
@@ -3140,17 +3179,17 @@
       <c r="F25" s="33">
         <v>0</v>
       </c>
-      <c r="H25" s="104" t="s">
+      <c r="H25" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="104"/>
-      <c r="J25" s="104"/>
-      <c r="K25" s="104"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104"/>
+      <c r="I25" s="125"/>
+      <c r="J25" s="125"/>
+      <c r="K25" s="125"/>
+      <c r="L25" s="125"/>
+      <c r="M25" s="125"/>
+      <c r="N25" s="125"/>
+      <c r="O25" s="125"/>
+      <c r="P25" s="125"/>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
@@ -3171,11 +3210,11 @@
       <c r="F26" s="66">
         <v>0</v>
       </c>
-      <c r="H26" s="104" t="s">
+      <c r="H26" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="125"/>
       <c r="K26">
         <f>(2*K18)+(2*K16)-(2*K17)</f>
         <v>57102</v>
@@ -3200,17 +3239,17 @@
       <c r="F27" s="68">
         <v>21</v>
       </c>
-      <c r="H27" s="104" t="s">
+      <c r="H27" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="I27" s="104"/>
-      <c r="J27" s="104"/>
-      <c r="K27" s="104"/>
-      <c r="L27" s="104"/>
-      <c r="M27" s="104"/>
-      <c r="N27" s="104"/>
-      <c r="O27" s="104"/>
-      <c r="P27" s="104"/>
+      <c r="I27" s="125"/>
+      <c r="J27" s="125"/>
+      <c r="K27" s="125"/>
+      <c r="L27" s="125"/>
+      <c r="M27" s="125"/>
+      <c r="N27" s="125"/>
+      <c r="O27" s="125"/>
+      <c r="P27" s="125"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -3231,61 +3270,61 @@
       <c r="F28" s="70">
         <v>11</v>
       </c>
-      <c r="H28" s="104" t="s">
+      <c r="H28" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="I28" s="104"/>
-      <c r="J28" s="104"/>
+      <c r="I28" s="125"/>
+      <c r="J28" s="125"/>
       <c r="K28">
         <f>(2*K18)+(2*K17)-(2*K16)</f>
         <v>52542</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H29" s="104" t="s">
+      <c r="H29" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="I29" s="104"/>
-      <c r="J29" s="104"/>
-      <c r="K29" s="104"/>
-      <c r="L29" s="104"/>
-      <c r="M29" s="104"/>
-      <c r="N29" s="104"/>
-      <c r="O29" s="104"/>
-      <c r="P29" s="104"/>
+      <c r="I29" s="125"/>
+      <c r="J29" s="125"/>
+      <c r="K29" s="125"/>
+      <c r="L29" s="125"/>
+      <c r="M29" s="125"/>
+      <c r="N29" s="125"/>
+      <c r="O29" s="125"/>
+      <c r="P29" s="125"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H30" s="104" t="s">
+      <c r="H30" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
+      <c r="I30" s="125"/>
+      <c r="J30" s="125"/>
       <c r="K30">
         <f>(2*K17)+(2*K18)-(2*K16)</f>
         <v>52542</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H31" s="104"/>
-      <c r="I31" s="104"/>
-      <c r="J31" s="104"/>
-      <c r="K31" s="104"/>
-      <c r="L31" s="104"/>
-      <c r="M31" s="104"/>
-      <c r="N31" s="104"/>
-      <c r="O31" s="104"/>
-      <c r="P31" s="104"/>
+      <c r="H31" s="125"/>
+      <c r="I31" s="125"/>
+      <c r="J31" s="125"/>
+      <c r="K31" s="125"/>
+      <c r="L31" s="125"/>
+      <c r="M31" s="125"/>
+      <c r="N31" s="125"/>
+      <c r="O31" s="125"/>
+      <c r="P31" s="125"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H33" s="104"/>
-      <c r="I33" s="104"/>
-      <c r="J33" s="104"/>
-      <c r="K33" s="104"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
-      <c r="O33" s="104"/>
-      <c r="P33" s="104"/>
+      <c r="H33" s="125"/>
+      <c r="I33" s="125"/>
+      <c r="J33" s="125"/>
+      <c r="K33" s="125"/>
+      <c r="L33" s="125"/>
+      <c r="M33" s="125"/>
+      <c r="N33" s="125"/>
+      <c r="O33" s="125"/>
+      <c r="P33" s="125"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -3302,15 +3341,15 @@
       <c r="B35" t="s">
         <v>133</v>
       </c>
-      <c r="H35" s="104"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="104"/>
-      <c r="K35" s="104"/>
-      <c r="L35" s="104"/>
-      <c r="M35" s="104"/>
-      <c r="N35" s="104"/>
-      <c r="O35" s="104"/>
-      <c r="P35" s="104"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="125"/>
+      <c r="K35" s="125"/>
+      <c r="L35" s="125"/>
+      <c r="M35" s="125"/>
+      <c r="N35" s="125"/>
+      <c r="O35" s="125"/>
+      <c r="P35" s="125"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -3358,6 +3397,21 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="H15:P15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:P21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="H25:P25"/>
+    <mergeCell ref="H26:J26"/>
     <mergeCell ref="H27:P27"/>
     <mergeCell ref="H29:P29"/>
     <mergeCell ref="H31:P31"/>
@@ -3365,21 +3419,6 @@
     <mergeCell ref="H35:P35"/>
     <mergeCell ref="H28:J28"/>
     <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H23:P23"/>
-    <mergeCell ref="H25:P25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:P21"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="H15:P15"/>
-    <mergeCell ref="H16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -3394,7 +3433,7 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -3569,34 +3608,34 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="126" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
+      <c r="C15" s="126"/>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3614,7 +3653,7 @@
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
   </cols>
@@ -4090,14 +4129,14 @@
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="125" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="125"/>
+      <c r="F27" s="125"/>
+      <c r="G27" s="125"/>
+      <c r="H27" s="125"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
@@ -4443,35 +4482,35 @@
       <c r="B52" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="104" t="s">
+      <c r="C52" s="125" t="s">
         <v>136</v>
       </c>
-      <c r="D52" s="104"/>
-      <c r="E52" s="104"/>
-      <c r="F52" s="104"/>
+      <c r="D52" s="125"/>
+      <c r="E52" s="125"/>
+      <c r="F52" s="125"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="104" t="s">
+      <c r="C53" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="104"/>
-      <c r="E53" s="104"/>
-      <c r="F53" s="104"/>
+      <c r="D53" s="125"/>
+      <c r="E53" s="125"/>
+      <c r="F53" s="125"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="104" t="s">
+      <c r="C54" s="125" t="s">
         <v>139</v>
       </c>
-      <c r="D54" s="104"/>
-      <c r="E54" s="104"/>
-      <c r="F54" s="104"/>
-      <c r="G54" s="104"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="125"/>
+      <c r="F54" s="125"/>
+      <c r="G54" s="125"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -4528,7 +4567,7 @@
       <selection activeCell="A26" sqref="A26:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
@@ -4698,14 +4737,14 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="104" t="s">
+      <c r="H9" s="125" t="s">
         <v>106</v>
       </c>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="125"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="125"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
@@ -4812,10 +4851,10 @@
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="111" t="s">
+      <c r="D16" s="106" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="29" t="s">
@@ -4830,16 +4869,16 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="112">
+      <c r="C17" s="107">
         <v>270</v>
       </c>
-      <c r="D17" s="113">
+      <c r="D17" s="108">
         <v>128</v>
       </c>
-      <c r="E17" s="110">
+      <c r="E17" s="105">
         <v>106</v>
       </c>
       <c r="I17" t="s">
@@ -4851,16 +4890,16 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="114">
+      <c r="C18" s="109">
         <v>128</v>
       </c>
-      <c r="D18" s="115">
+      <c r="D18" s="110">
         <v>234</v>
       </c>
-      <c r="E18" s="116">
+      <c r="E18" s="111">
         <v>67</v>
       </c>
       <c r="I18" t="s">
@@ -4881,7 +4920,7 @@
       <c r="D19" s="65">
         <v>67</v>
       </c>
-      <c r="E19" s="117">
+      <c r="E19" s="112">
         <v>173</v>
       </c>
       <c r="I19" t="s">
@@ -4893,21 +4932,21 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="105" t="s">
+      <c r="C22" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="126"/>
+      <c r="E24" s="126"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -4986,7 +5025,7 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
@@ -5166,10 +5205,10 @@
         <v>59</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="111" t="s">
+      <c r="J10" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="111" t="s">
+      <c r="K10" s="106" t="s">
         <v>56</v>
       </c>
       <c r="L10" s="29" t="s">
@@ -5195,16 +5234,16 @@
       <c r="F11" s="3">
         <v>15</v>
       </c>
-      <c r="I11" s="109" t="s">
+      <c r="I11" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="112">
+      <c r="J11" s="107">
         <v>30</v>
       </c>
-      <c r="K11" s="113">
+      <c r="K11" s="108">
         <v>30</v>
       </c>
-      <c r="L11" s="110">
+      <c r="L11" s="105">
         <v>0</v>
       </c>
       <c r="M11" s="3">
@@ -5227,16 +5266,16 @@
       <c r="F12" s="3">
         <v>45</v>
       </c>
-      <c r="I12" s="109" t="s">
+      <c r="I12" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="114">
+      <c r="J12" s="109">
         <v>30</v>
       </c>
-      <c r="K12" s="115">
+      <c r="K12" s="110">
         <v>45</v>
       </c>
-      <c r="L12" s="116">
+      <c r="L12" s="111">
         <v>0</v>
       </c>
       <c r="M12" s="66">
@@ -5268,10 +5307,10 @@
       <c r="K13" s="65">
         <v>0</v>
       </c>
-      <c r="L13" s="118">
+      <c r="L13" s="113">
         <v>45</v>
       </c>
-      <c r="M13" s="119">
+      <c r="M13" s="114">
         <v>45</v>
       </c>
     </row>
@@ -5300,10 +5339,10 @@
       <c r="K14" s="46">
         <v>15</v>
       </c>
-      <c r="L14" s="120">
+      <c r="L14" s="115">
         <v>45</v>
       </c>
-      <c r="M14" s="121">
+      <c r="M14" s="116">
         <v>65</v>
       </c>
     </row>
@@ -5380,7 +5419,7 @@
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="4.140625" customWidth="1"/>
@@ -5663,15 +5702,15 @@
       <c r="H12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="104" t="s">
+      <c r="K12" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="104"/>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="104"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="125"/>
+      <c r="N12" s="125"/>
+      <c r="O12" s="125"/>
+      <c r="P12" s="125"/>
+      <c r="Q12" s="125"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="60" t="s">
@@ -5701,11 +5740,11 @@
         <f>O6+O7+O8</f>
         <v>587</v>
       </c>
-      <c r="L13" s="104" t="s">
+      <c r="L13" s="125" t="s">
         <v>117</v>
       </c>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104"/>
+      <c r="M13" s="125"/>
+      <c r="N13" s="125"/>
       <c r="O13">
         <f>C13*F13+C14*F14+C15*F15+C16*F16+C17*F17+C18*F18</f>
         <v>1710503</v>
@@ -5739,11 +5778,11 @@
         <f>O7+O8</f>
         <v>415</v>
       </c>
-      <c r="L14" s="104" t="s">
+      <c r="L14" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
+      <c r="M14" s="125"/>
+      <c r="N14" s="125"/>
       <c r="O14">
         <f>F13*H13+F14*H14+F15*H15+F16*H16+F17*H17+F18*H18</f>
         <v>1550382</v>
@@ -5777,11 +5816,11 @@
         <f>O7+O8</f>
         <v>415</v>
       </c>
-      <c r="L15" s="104" t="s">
+      <c r="L15" s="125" t="s">
         <v>119</v>
       </c>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
+      <c r="M15" s="125"/>
+      <c r="N15" s="125"/>
       <c r="O15">
         <f>C13*H13+C14*H14+C15*H15+C16*H16+C17*H17+C18*H18</f>
         <v>1710503</v>
@@ -5844,11 +5883,11 @@
         <f>O7+O8</f>
         <v>415</v>
       </c>
-      <c r="L17" s="104" t="s">
+      <c r="L17" s="125" t="s">
         <v>115</v>
       </c>
-      <c r="M17" s="104"/>
-      <c r="N17" s="104"/>
+      <c r="M17" s="125"/>
+      <c r="N17" s="125"/>
       <c r="O17">
         <f>2*O13+2*O14-2*O15</f>
         <v>3100764</v>
@@ -5882,44 +5921,44 @@
         <f>O6+O7+O8</f>
         <v>587</v>
       </c>
-      <c r="L18" s="104" t="s">
+      <c r="L18" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="M18" s="104"/>
-      <c r="N18" s="104"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
       <c r="O18">
         <f>2*O15+2*O14-2*O13</f>
         <v>3100764</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L19" s="104" t="s">
+      <c r="L19" s="125" t="s">
         <v>121</v>
       </c>
-      <c r="M19" s="104"/>
-      <c r="N19" s="104"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="125"/>
       <c r="O19">
         <f>2*O13+2*O15-2*O14</f>
         <v>3741248</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L20" s="104" t="s">
+      <c r="L20" s="125" t="s">
         <v>122</v>
       </c>
-      <c r="M20" s="104"/>
-      <c r="N20" s="104"/>
+      <c r="M20" s="125"/>
+      <c r="N20" s="125"/>
       <c r="O20">
         <f>2*O14+2*O15-2*O13</f>
         <v>3100764</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="104" t="s">
+      <c r="L21" s="125" t="s">
         <v>123</v>
       </c>
-      <c r="M21" s="104"/>
-      <c r="N21" s="104"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
       <c r="O21">
         <f>2*O14+2*O13-2*O15</f>
         <v>3100764</v>
@@ -5927,13 +5966,13 @@
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="111" t="s">
+      <c r="C22" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="111" t="s">
+      <c r="D22" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="106" t="s">
         <v>61</v>
       </c>
       <c r="F22" s="29" t="s">
@@ -5945,33 +5984,33 @@
       <c r="H22" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="104" t="s">
+      <c r="L22" s="125" t="s">
         <v>124</v>
       </c>
-      <c r="M22" s="104"/>
-      <c r="N22" s="104"/>
+      <c r="M22" s="125"/>
+      <c r="N22" s="125"/>
       <c r="O22">
         <f>2*O15+2*O13-2*O14</f>
         <v>3741248</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="112">
+      <c r="C23" s="107">
         <f>F16</f>
         <v>587</v>
       </c>
-      <c r="D23" s="122">
+      <c r="D23" s="117">
         <f>F13</f>
         <v>587</v>
       </c>
-      <c r="E23" s="113">
+      <c r="E23" s="108">
         <f>F18</f>
         <v>587</v>
       </c>
-      <c r="F23" s="110">
+      <c r="F23" s="105">
         <f>F14</f>
         <v>415</v>
       </c>
@@ -5985,10 +6024,10 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="123">
+      <c r="C24" s="118">
         <f>F13</f>
         <v>587</v>
       </c>
@@ -5996,11 +6035,11 @@
         <f>C13</f>
         <v>700</v>
       </c>
-      <c r="E24" s="124">
+      <c r="E24" s="119">
         <f>H13</f>
         <v>587</v>
       </c>
-      <c r="F24" s="110">
+      <c r="F24" s="105">
         <f>D16</f>
         <v>415</v>
       </c>
@@ -6014,22 +6053,22 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="114">
+      <c r="C25" s="109">
         <f>F18</f>
         <v>587</v>
       </c>
-      <c r="D25" s="125">
+      <c r="D25" s="120">
         <f>H13</f>
         <v>587</v>
       </c>
-      <c r="E25" s="115">
+      <c r="E25" s="110">
         <f>H18</f>
         <v>587</v>
       </c>
-      <c r="F25" s="116">
+      <c r="F25" s="111">
         <f>H14</f>
         <v>415</v>
       </c>
@@ -6058,15 +6097,15 @@
         <f>H14</f>
         <v>415</v>
       </c>
-      <c r="F26" s="118">
+      <c r="F26" s="113">
         <f>D14</f>
         <v>679</v>
       </c>
-      <c r="G26" s="126">
+      <c r="G26" s="121">
         <f>D15</f>
         <v>415</v>
       </c>
-      <c r="H26" s="119">
+      <c r="H26" s="114">
         <f>D17</f>
         <v>679</v>
       </c>
@@ -6087,7 +6126,7 @@
         <f>H15</f>
         <v>415</v>
       </c>
-      <c r="F27" s="127">
+      <c r="F27" s="122">
         <f>E14</f>
         <v>415</v>
       </c>
@@ -6095,7 +6134,7 @@
         <f>E15</f>
         <v>415</v>
       </c>
-      <c r="H27" s="128">
+      <c r="H27" s="123">
         <f>E17</f>
         <v>415</v>
       </c>
@@ -6122,15 +6161,15 @@
         <f>H17</f>
         <v>415</v>
       </c>
-      <c r="F28" s="120">
+      <c r="F28" s="115">
         <f>G14</f>
         <v>679</v>
       </c>
-      <c r="G28" s="129">
+      <c r="G28" s="124">
         <f>G15</f>
         <v>415</v>
       </c>
-      <c r="H28" s="121">
+      <c r="H28" s="116">
         <f>G17</f>
         <v>679</v>
       </c>
@@ -6187,16 +6226,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="L22:N22"/>
     <mergeCell ref="L13:N13"/>
     <mergeCell ref="K12:Q12"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="L22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6210,7 +6249,7 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
     <col min="3" max="3" width="3.140625" customWidth="1"/>
@@ -6770,16 +6809,16 @@
       <c r="L15" s="56">
         <v>0</v>
       </c>
-      <c r="P15" s="104" t="s">
+      <c r="P15" s="125" t="s">
         <v>150</v>
       </c>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="104"/>
-      <c r="V15" s="104"/>
-      <c r="W15" s="104"/>
+      <c r="Q15" s="125"/>
+      <c r="R15" s="125"/>
+      <c r="S15" s="125"/>
+      <c r="T15" s="125"/>
+      <c r="U15" s="125"/>
+      <c r="V15" s="125"/>
+      <c r="W15" s="125"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" s="60" t="s">
@@ -6817,12 +6856,12 @@
       <c r="L16" s="56">
         <v>0</v>
       </c>
-      <c r="P16" s="104" t="s">
+      <c r="P16" s="125" t="s">
         <v>157</v>
       </c>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
+      <c r="Q16" s="125"/>
+      <c r="R16" s="125"/>
+      <c r="S16" s="125"/>
       <c r="T16">
         <f>G15*J15+G16*J16+G17*J17+G18*J18+G19*J19+G20*J20+G21*J21+G22*J22+G23*J23+G24*J24</f>
         <v>16000</v>
@@ -6863,12 +6902,12 @@
       <c r="L17" s="56">
         <v>15</v>
       </c>
-      <c r="P17" s="104" t="s">
+      <c r="P17" s="125" t="s">
         <v>158</v>
       </c>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
+      <c r="Q17" s="125"/>
+      <c r="R17" s="125"/>
+      <c r="S17" s="125"/>
       <c r="T17">
         <f>J15*K15+J16*K16+J17*K17+J18*K18+J19*K19+J20*K20+J21*K21+J22*K22+J23*K23+J24*K24</f>
         <v>36500</v>
@@ -6909,12 +6948,12 @@
       <c r="L18" s="56">
         <v>40</v>
       </c>
-      <c r="P18" s="104" t="s">
+      <c r="P18" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="Q18" s="104"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
+      <c r="Q18" s="125"/>
+      <c r="R18" s="125"/>
+      <c r="S18" s="125"/>
       <c r="T18">
         <f>J15*K15+J16*K16+J17*K17+J18*K18+J19*K19+J20*K20+J21*K21+J22*K22+J23*K23+J24*K24</f>
         <v>36500</v>
@@ -6991,12 +7030,12 @@
       <c r="L20" s="56">
         <v>40</v>
       </c>
-      <c r="Q20" s="104" t="s">
+      <c r="Q20" s="125" t="s">
         <v>151</v>
       </c>
-      <c r="R20" s="104"/>
-      <c r="S20" s="104"/>
-      <c r="T20" s="104"/>
+      <c r="R20" s="125"/>
+      <c r="S20" s="125"/>
+      <c r="T20" s="125"/>
       <c r="U20">
         <f>2*T16+2*T17-2*T18</f>
         <v>32000</v>
@@ -7037,12 +7076,12 @@
       <c r="L21" s="56">
         <v>0</v>
       </c>
-      <c r="Q21" s="104" t="s">
+      <c r="Q21" s="125" t="s">
         <v>152</v>
       </c>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="104"/>
+      <c r="R21" s="125"/>
+      <c r="S21" s="125"/>
+      <c r="T21" s="125"/>
       <c r="U21">
         <f>2*T18+2*T17-2*T16</f>
         <v>114000</v>
@@ -7083,12 +7122,12 @@
       <c r="L22" s="56">
         <v>0</v>
       </c>
-      <c r="Q22" s="104" t="s">
+      <c r="Q22" s="125" t="s">
         <v>153</v>
       </c>
-      <c r="R22" s="104"/>
-      <c r="S22" s="104"/>
-      <c r="T22" s="104"/>
+      <c r="R22" s="125"/>
+      <c r="S22" s="125"/>
+      <c r="T22" s="125"/>
       <c r="U22">
         <f>2*T16+2*T18-2*T17</f>
         <v>32000</v>
@@ -7129,12 +7168,12 @@
       <c r="L23" s="56">
         <v>15</v>
       </c>
-      <c r="Q23" s="104" t="s">
+      <c r="Q23" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="R23" s="104"/>
-      <c r="S23" s="104"/>
-      <c r="T23" s="104"/>
+      <c r="R23" s="125"/>
+      <c r="S23" s="125"/>
+      <c r="T23" s="125"/>
       <c r="U23">
         <f>2*T17+2*T18-2*T16</f>
         <v>114000</v>
@@ -7175,24 +7214,24 @@
         <f>S6+S11</f>
         <v>40</v>
       </c>
-      <c r="Q24" s="104" t="s">
+      <c r="Q24" s="125" t="s">
         <v>155</v>
       </c>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
+      <c r="R24" s="125"/>
+      <c r="S24" s="125"/>
+      <c r="T24" s="125"/>
       <c r="U24">
         <f>2*T17+2*T16-2*T18</f>
         <v>32000</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="Q25" s="104" t="s">
+      <c r="Q25" s="125" t="s">
         <v>156</v>
       </c>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="104"/>
+      <c r="R25" s="125"/>
+      <c r="S25" s="125"/>
+      <c r="T25" s="125"/>
       <c r="U25">
         <f>2*T18+2*T16-2*T17</f>
         <v>32000</v>
@@ -7427,16 +7466,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="P18:S18"/>
+    <mergeCell ref="P15:W15"/>
+    <mergeCell ref="Q20:T20"/>
     <mergeCell ref="Q21:T21"/>
     <mergeCell ref="Q22:T22"/>
     <mergeCell ref="Q23:T23"/>
     <mergeCell ref="Q24:T24"/>
     <mergeCell ref="Q25:T25"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="P18:S18"/>
-    <mergeCell ref="P15:W15"/>
-    <mergeCell ref="Q20:T20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7450,7 +7489,7 @@
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" customWidth="1"/>
@@ -7777,7 +7816,7 @@
       <selection activeCell="F28" sqref="F28:K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -7916,14 +7955,14 @@
       <c r="D9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="104" t="s">
+      <c r="F9" s="125" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="125"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -7938,14 +7977,14 @@
       <c r="D10" s="3">
         <v>15</v>
       </c>
-      <c r="F10" s="104" t="s">
+      <c r="F10" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="125"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -7960,14 +7999,14 @@
       <c r="D11" s="3">
         <v>35</v>
       </c>
-      <c r="F11" s="104" t="s">
+      <c r="F11" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
+      <c r="G11" s="125"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="125"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
@@ -7982,107 +8021,112 @@
       <c r="D12" s="3">
         <v>50</v>
       </c>
-      <c r="F12" s="104" t="s">
+      <c r="F12" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
+      <c r="G12" s="125"/>
+      <c r="H12" s="125"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="125"/>
+      <c r="K12" s="125"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="104" t="s">
+      <c r="F14" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
+      <c r="G14" s="125"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125"/>
+      <c r="K14" s="125"/>
     </row>
     <row r="19" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F19" s="104" t="s">
+      <c r="F19" s="125" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="104"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="104"/>
-      <c r="K19" s="104"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="125"/>
     </row>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="104" t="s">
+      <c r="F20" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="104"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="104"/>
-      <c r="J20" s="104"/>
-      <c r="K20" s="104"/>
+      <c r="G20" s="125"/>
+      <c r="H20" s="125"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
+      <c r="K20" s="125"/>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="104" t="s">
+      <c r="F21" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="104"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="125"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="125"/>
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="104" t="s">
+      <c r="F22" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="104"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="104"/>
-      <c r="J22" s="104"/>
-      <c r="K22" s="104"/>
+      <c r="G22" s="125"/>
+      <c r="H22" s="125"/>
+      <c r="I22" s="125"/>
+      <c r="J22" s="125"/>
+      <c r="K22" s="125"/>
     </row>
     <row r="27" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F27" s="104" t="s">
+      <c r="F27" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104"/>
-      <c r="I27" s="104"/>
-      <c r="J27" s="104"/>
-      <c r="K27" s="104"/>
+      <c r="G27" s="125"/>
+      <c r="H27" s="125"/>
+      <c r="I27" s="125"/>
+      <c r="J27" s="125"/>
+      <c r="K27" s="125"/>
     </row>
     <row r="28" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="104" t="s">
+      <c r="F28" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="104"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="104"/>
-      <c r="K28" s="104"/>
+      <c r="G28" s="125"/>
+      <c r="H28" s="125"/>
+      <c r="I28" s="125"/>
+      <c r="J28" s="125"/>
+      <c r="K28" s="125"/>
     </row>
     <row r="29" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F29" s="104" t="s">
+      <c r="F29" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="104"/>
-      <c r="H29" s="104"/>
-      <c r="I29" s="104"/>
-      <c r="J29" s="104"/>
-      <c r="K29" s="104"/>
+      <c r="G29" s="125"/>
+      <c r="H29" s="125"/>
+      <c r="I29" s="125"/>
+      <c r="J29" s="125"/>
+      <c r="K29" s="125"/>
     </row>
     <row r="30" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F30" s="104" t="s">
+      <c r="F30" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="104"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
-      <c r="K30" s="104"/>
+      <c r="G30" s="125"/>
+      <c r="H30" s="125"/>
+      <c r="I30" s="125"/>
+      <c r="J30" s="125"/>
+      <c r="K30" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F9:K9"/>
+    <mergeCell ref="F10:K10"/>
+    <mergeCell ref="F11:K11"/>
+    <mergeCell ref="F12:K12"/>
+    <mergeCell ref="F19:K19"/>
     <mergeCell ref="F30:K30"/>
     <mergeCell ref="F14:K14"/>
     <mergeCell ref="F22:K22"/>
@@ -8091,11 +8135,6 @@
     <mergeCell ref="F27:K27"/>
     <mergeCell ref="F29:K29"/>
     <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F9:K9"/>
-    <mergeCell ref="F10:K10"/>
-    <mergeCell ref="F11:K11"/>
-    <mergeCell ref="F12:K12"/>
-    <mergeCell ref="F19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>